<commit_message>
Update bad cluster spreadsheets
Some khipus had bad clusters which is noted in excel file
</commit_message>
<xml_diff>
--- a/data/KFG_DB_Excel/AS012.xlsx
+++ b/data/KFG_DB_Excel/AS012.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="273">
   <si>
     <t>!-----------------------------------------------------------------------------------------------</t>
   </si>
@@ -120,13 +120,13 @@
     <t>Region:Unknown</t>
   </si>
   <si>
-    <t>Notes:1. Construction note: MB is joined to W at 7 cm. consistantly.&lt;br/&gt;2. No numbers or subsidiaries appear on the last 41 pendants which are separated from the first 44 pendants by the knot on the main cord.&lt;br/&gt;3. Grouping is by color: groups 1, 2, 3 are MB, MB/W, W respectively, and this is repeated in groups 4, 5, 6.</t>
+    <t>Notes:</t>
   </si>
   <si>
     <t>Creation_Date:5/24/12 13:33</t>
   </si>
   <si>
-    <t>Excel Write Date:2023-05-29</t>
+    <t>Excel Write Date:2023-06-07</t>
   </si>
   <si>
     <t>Excel File Creator:Ashok Khosla</t>
@@ -159,34 +159,31 @@
     <t>Twist:U</t>
   </si>
   <si>
-    <t>Notes:</t>
-  </si>
-  <si>
     <t>Plain_Notes:</t>
   </si>
   <si>
     <t>!-- Pendant Data</t>
   </si>
   <si>
-    <t>0.0cm group of 9 pendants (1-9) space of 0.0cm</t>
-  </si>
-  <si>
-    <t>3.0cm group of 12 pendants (10-21) space of 0.0cm</t>
-  </si>
-  <si>
-    <t>7.0cm group of 23 pendants (22-44) space of 0.0cm</t>
-  </si>
-  <si>
-    <t>7.0cm 12 (45)</t>
-  </si>
-  <si>
-    <t>15.0cm group of 12 pendants (46-57) space of 0.0cm</t>
-  </si>
-  <si>
-    <t>18.0cm group of 17 pendants (58-69) space of 0.0cm</t>
-  </si>
-  <si>
-    <t>22.0cm group of 0 pendants (70-86) space of 0.0cm</t>
+    <t>0.1cm group of 9 pendants (1-9) space of 0.1cm</t>
+  </si>
+  <si>
+    <t>3.0cm group of 12 pendants (10-21) space of 0.1cm</t>
+  </si>
+  <si>
+    <t>7.0cm group of 23 pendants (22-44) space of 0.1cm</t>
+  </si>
+  <si>
+    <t>7.0cm 1 (45)</t>
+  </si>
+  <si>
+    <t>15.0cm group of 12 pendants (46-57) space of 0.1cm</t>
+  </si>
+  <si>
+    <t>18.0cm group of 12 pendants (58-69) space of 0.1cm</t>
+  </si>
+  <si>
+    <t>22.0cm group of 16 pendants (70-85) space of 0.1cm</t>
   </si>
   <si>
     <t>Cord_Name</t>
@@ -652,6 +649,9 @@
   </si>
   <si>
     <t>p41</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
   <si>
     <t>p42</t>
@@ -1433,12 +1433,12 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1456,42 +1456,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1509,1723 +1509,1726 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>65</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>66</v>
-      </c>
-      <c r="L1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>70</v>
       </c>
-      <c r="F2" t="s">
-        <v>71</v>
-      </c>
       <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
         <v>72</v>
       </c>
-      <c r="H2" t="s">
-        <v>73</v>
-      </c>
       <c r="I2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>76</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>77</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" t="s">
         <v>78</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>81</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
         <v>82</v>
       </c>
-      <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>83</v>
-      </c>
-      <c r="K4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
         <v>85</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>86</v>
-      </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="s">
-        <v>73</v>
-      </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>88</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
         <v>89</v>
-      </c>
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" t="s">
         <v>72</v>
       </c>
-      <c r="H7" t="s">
-        <v>73</v>
-      </c>
       <c r="I7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
         <v>93</v>
       </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>94</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" t="s">
         <v>95</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
         <v>97</v>
       </c>
-      <c r="B9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E9" t="s">
-        <v>98</v>
-      </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" t="s">
         <v>72</v>
       </c>
-      <c r="H9" t="s">
-        <v>73</v>
-      </c>
       <c r="I9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
         <v>99</v>
       </c>
-      <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" t="s">
-        <v>100</v>
-      </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
         <v>72</v>
       </c>
-      <c r="H10" t="s">
-        <v>73</v>
-      </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" t="s">
-        <v>102</v>
-      </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
         <v>103</v>
       </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" t="s">
-        <v>104</v>
-      </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" t="s">
         <v>72</v>
       </c>
-      <c r="H12" t="s">
-        <v>73</v>
-      </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
         <v>105</v>
       </c>
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>106</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" t="s">
         <v>107</v>
       </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" t="s">
-        <v>108</v>
-      </c>
       <c r="I13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" t="s">
         <v>107</v>
       </c>
-      <c r="F14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" t="s">
-        <v>108</v>
-      </c>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
         <v>110</v>
       </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" t="s">
         <v>111</v>
-      </c>
-      <c r="E15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" t="s">
         <v>107</v>
       </c>
-      <c r="F16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" t="s">
-        <v>108</v>
-      </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
         <v>114</v>
       </c>
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" t="s">
         <v>115</v>
       </c>
-      <c r="F17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" t="s">
-        <v>72</v>
-      </c>
-      <c r="H17" t="s">
-        <v>116</v>
-      </c>
       <c r="I17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
         <v>117</v>
       </c>
-      <c r="B18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" t="s">
         <v>118</v>
-      </c>
-      <c r="F18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" t="s">
-        <v>74</v>
-      </c>
-      <c r="K18" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
         <v>120</v>
       </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" t="s">
-        <v>121</v>
-      </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
         <v>122</v>
       </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>123</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
         <v>124</v>
       </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" t="s">
-        <v>125</v>
-      </c>
       <c r="I20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" t="s">
         <v>115</v>
       </c>
-      <c r="F21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" t="s">
-        <v>116</v>
-      </c>
       <c r="I21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
         <v>127</v>
       </c>
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I22" t="s">
         <v>128</v>
       </c>
-      <c r="E22" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" t="s">
-        <v>116</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>129</v>
-      </c>
-      <c r="K22" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" t="s">
         <v>132</v>
       </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" t="s">
-        <v>133</v>
-      </c>
       <c r="I24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
         <v>134</v>
       </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
         <v>135</v>
       </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" t="s">
-        <v>136</v>
-      </c>
       <c r="I25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" t="s">
         <v>124</v>
       </c>
-      <c r="F26" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" t="s">
-        <v>72</v>
-      </c>
-      <c r="H26" t="s">
-        <v>125</v>
-      </c>
       <c r="I26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
         <v>138</v>
       </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>139</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" t="s">
         <v>140</v>
       </c>
-      <c r="F27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>141</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>142</v>
-      </c>
-      <c r="K27" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" t="s">
         <v>145</v>
       </c>
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" t="s">
         <v>146</v>
       </c>
-      <c r="F29" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" t="s">
-        <v>147</v>
-      </c>
       <c r="I29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" t="s">
         <v>148</v>
       </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" t="s">
-        <v>123</v>
-      </c>
-      <c r="E30" t="s">
-        <v>149</v>
-      </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
         <v>150</v>
       </c>
-      <c r="B31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>151</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
+        <v>146</v>
+      </c>
+      <c r="I31" t="s">
         <v>152</v>
-      </c>
-      <c r="F31" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" t="s">
-        <v>72</v>
-      </c>
-      <c r="H31" t="s">
-        <v>147</v>
-      </c>
-      <c r="I31" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
         <v>155</v>
       </c>
-      <c r="B33" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" t="s">
-        <v>156</v>
-      </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" t="s">
-        <v>70</v>
-      </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
         <v>158</v>
       </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" t="s">
+        <v>146</v>
+      </c>
+      <c r="I35" t="s">
         <v>159</v>
       </c>
-      <c r="E35" t="s">
-        <v>149</v>
-      </c>
-      <c r="F35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" t="s">
-        <v>72</v>
-      </c>
-      <c r="H35" t="s">
-        <v>147</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>160</v>
-      </c>
-      <c r="K35" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" t="s">
         <v>162</v>
       </c>
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" t="s">
-        <v>163</v>
-      </c>
       <c r="F36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" t="s">
         <v>72</v>
       </c>
-      <c r="H37" t="s">
-        <v>73</v>
-      </c>
       <c r="I37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H38" t="s">
         <v>72</v>
       </c>
-      <c r="H38" t="s">
-        <v>73</v>
-      </c>
       <c r="I38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" t="s">
         <v>166</v>
       </c>
-      <c r="B39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" t="s">
-        <v>167</v>
-      </c>
       <c r="F39" t="s">
+        <v>77</v>
+      </c>
+      <c r="G39" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" t="s">
+        <v>146</v>
+      </c>
+      <c r="I39" t="s">
         <v>78</v>
-      </c>
-      <c r="G39" t="s">
-        <v>72</v>
-      </c>
-      <c r="H39" t="s">
-        <v>147</v>
-      </c>
-      <c r="I39" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" t="s">
         <v>168</v>
       </c>
-      <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>169</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" t="s">
+        <v>146</v>
+      </c>
+      <c r="I40" t="s">
         <v>170</v>
-      </c>
-      <c r="F40" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40" t="s">
-        <v>72</v>
-      </c>
-      <c r="H40" t="s">
-        <v>147</v>
-      </c>
-      <c r="I40" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
         <v>172</v>
       </c>
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>173</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" t="s">
+        <v>71</v>
+      </c>
+      <c r="H41" t="s">
+        <v>146</v>
+      </c>
+      <c r="I41" t="s">
         <v>174</v>
       </c>
-      <c r="F41" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" t="s">
-        <v>72</v>
-      </c>
-      <c r="H41" t="s">
-        <v>147</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>175</v>
-      </c>
-      <c r="K41" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" t="s">
         <v>177</v>
       </c>
-      <c r="B42" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" t="s">
-        <v>178</v>
-      </c>
       <c r="F42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G44" t="s">
+        <v>71</v>
+      </c>
+      <c r="H44" t="s">
+        <v>146</v>
+      </c>
+      <c r="I44" t="s">
+        <v>159</v>
+      </c>
+      <c r="K44" t="s">
         <v>180</v>
-      </c>
-      <c r="B44" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" t="s">
-        <v>69</v>
-      </c>
-      <c r="D44" t="s">
-        <v>159</v>
-      </c>
-      <c r="E44" t="s">
-        <v>115</v>
-      </c>
-      <c r="F44" t="s">
-        <v>78</v>
-      </c>
-      <c r="G44" t="s">
-        <v>72</v>
-      </c>
-      <c r="H44" t="s">
-        <v>147</v>
-      </c>
-      <c r="I44" t="s">
-        <v>160</v>
-      </c>
-      <c r="K44" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" t="s">
         <v>182</v>
       </c>
-      <c r="B45" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" t="s">
-        <v>183</v>
-      </c>
       <c r="F45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" t="s">
+        <v>71</v>
+      </c>
+      <c r="H46" t="s">
+        <v>146</v>
+      </c>
+      <c r="I46" t="s">
         <v>159</v>
       </c>
-      <c r="E46" t="s">
-        <v>115</v>
-      </c>
-      <c r="F46" t="s">
-        <v>78</v>
-      </c>
-      <c r="G46" t="s">
-        <v>72</v>
-      </c>
-      <c r="H46" t="s">
-        <v>147</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="K46" t="s">
         <v>160</v>
-      </c>
-      <c r="K46" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" t="s">
         <v>185</v>
       </c>
-      <c r="B47" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" t="s">
-        <v>186</v>
-      </c>
       <c r="F47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" t="s">
         <v>187</v>
       </c>
-      <c r="B48" t="s">
-        <v>69</v>
-      </c>
-      <c r="C48" t="s">
-        <v>69</v>
-      </c>
-      <c r="E48" t="s">
-        <v>188</v>
-      </c>
       <c r="F48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48" t="s">
         <v>72</v>
       </c>
-      <c r="H48" t="s">
-        <v>73</v>
-      </c>
       <c r="I48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" t="s">
         <v>192</v>
       </c>
-      <c r="B52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" t="s">
-        <v>193</v>
-      </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" t="s">
         <v>69</v>
       </c>
-      <c r="C53" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>70</v>
       </c>
-      <c r="F53" t="s">
-        <v>71</v>
-      </c>
       <c r="G53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
+        <v>194</v>
+      </c>
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" t="s">
+        <v>68</v>
+      </c>
+      <c r="E54" t="s">
         <v>195</v>
       </c>
-      <c r="B54" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
+        <v>77</v>
+      </c>
+      <c r="G54" t="s">
+        <v>71</v>
+      </c>
+      <c r="H54" t="s">
+        <v>146</v>
+      </c>
+      <c r="I54" t="s">
+        <v>73</v>
+      </c>
+      <c r="K54" t="s">
         <v>196</v>
-      </c>
-      <c r="F54" t="s">
-        <v>78</v>
-      </c>
-      <c r="G54" t="s">
-        <v>72</v>
-      </c>
-      <c r="H54" t="s">
-        <v>147</v>
-      </c>
-      <c r="I54" t="s">
-        <v>74</v>
-      </c>
-      <c r="K54" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" t="s">
+        <v>173</v>
+      </c>
+      <c r="F55" t="s">
+        <v>77</v>
+      </c>
+      <c r="G55" t="s">
+        <v>71</v>
+      </c>
+      <c r="H55" t="s">
         <v>198</v>
       </c>
-      <c r="B55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" t="s">
-        <v>174</v>
-      </c>
-      <c r="F55" t="s">
-        <v>78</v>
-      </c>
-      <c r="G55" t="s">
-        <v>72</v>
-      </c>
-      <c r="H55" t="s">
-        <v>199</v>
-      </c>
       <c r="I55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
+        <v>199</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" t="s">
+        <v>122</v>
+      </c>
+      <c r="E56" t="s">
         <v>200</v>
       </c>
-      <c r="B56" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" t="s">
-        <v>201</v>
-      </c>
       <c r="F56" t="s">
+        <v>77</v>
+      </c>
+      <c r="G56" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" t="s">
+        <v>146</v>
+      </c>
+      <c r="I56" t="s">
         <v>78</v>
-      </c>
-      <c r="G56" t="s">
-        <v>72</v>
-      </c>
-      <c r="H56" t="s">
-        <v>147</v>
-      </c>
-      <c r="I56" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
+        <v>201</v>
+      </c>
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" t="s">
         <v>202</v>
       </c>
-      <c r="B57" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" t="s">
-        <v>123</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
+        <v>77</v>
+      </c>
+      <c r="G57" t="s">
+        <v>71</v>
+      </c>
+      <c r="H57" t="s">
+        <v>146</v>
+      </c>
+      <c r="I57" t="s">
+        <v>78</v>
+      </c>
+      <c r="K57" t="s">
         <v>203</v>
-      </c>
-      <c r="F57" t="s">
-        <v>78</v>
-      </c>
-      <c r="G57" t="s">
-        <v>72</v>
-      </c>
-      <c r="H57" t="s">
-        <v>147</v>
-      </c>
-      <c r="I57" t="s">
-        <v>79</v>
-      </c>
-      <c r="K57" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" t="s">
         <v>205</v>
       </c>
-      <c r="B58" t="s">
-        <v>69</v>
-      </c>
-      <c r="C58" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" t="s">
-        <v>206</v>
-      </c>
       <c r="F58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G58" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" t="s">
         <v>72</v>
       </c>
-      <c r="H58" t="s">
-        <v>73</v>
-      </c>
       <c r="I58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
+        <v>207</v>
+      </c>
+      <c r="B60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" t="s">
+        <v>68</v>
+      </c>
+      <c r="E60" t="s">
         <v>208</v>
       </c>
-      <c r="B60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60" t="s">
-        <v>69</v>
-      </c>
-      <c r="E60" t="s">
-        <v>209</v>
-      </c>
       <c r="F60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
+        <v>209</v>
+      </c>
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" t="s">
+        <v>75</v>
+      </c>
+      <c r="E61" t="s">
+        <v>145</v>
+      </c>
+      <c r="F61" t="s">
+        <v>77</v>
+      </c>
+      <c r="G61" t="s">
+        <v>71</v>
+      </c>
+      <c r="H61" t="s">
         <v>210</v>
       </c>
-      <c r="B61" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" t="s">
-        <v>69</v>
-      </c>
-      <c r="D61" t="s">
-        <v>76</v>
-      </c>
-      <c r="E61" t="s">
-        <v>146</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="I61" t="s">
         <v>78</v>
-      </c>
-      <c r="G61" t="s">
-        <v>72</v>
-      </c>
-      <c r="I61" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3233,28 +3236,31 @@
         <v>211</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" t="s">
         <v>212</v>
       </c>
       <c r="E62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G62" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="H62" t="s">
+        <v>210</v>
       </c>
       <c r="I62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3262,25 +3268,25 @@
         <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3288,25 +3294,25 @@
         <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E64" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3314,25 +3320,25 @@
         <v>215</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E65" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3340,25 +3346,25 @@
         <v>216</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66" t="s">
         <v>72</v>
       </c>
-      <c r="H66" t="s">
-        <v>73</v>
-      </c>
       <c r="I66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3366,25 +3372,25 @@
         <v>217</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G67" t="s">
+        <v>71</v>
+      </c>
+      <c r="H67" t="s">
         <v>72</v>
       </c>
-      <c r="H67" t="s">
-        <v>73</v>
-      </c>
       <c r="I67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3392,25 +3398,25 @@
         <v>218</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G68" t="s">
+        <v>71</v>
+      </c>
+      <c r="H68" t="s">
         <v>72</v>
       </c>
-      <c r="H68" t="s">
-        <v>73</v>
-      </c>
       <c r="I68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3418,25 +3424,25 @@
         <v>219</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G69" t="s">
+        <v>71</v>
+      </c>
+      <c r="H69" t="s">
         <v>72</v>
       </c>
-      <c r="H69" t="s">
-        <v>73</v>
-      </c>
       <c r="I69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3444,25 +3450,25 @@
         <v>220</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G70" t="s">
+        <v>71</v>
+      </c>
+      <c r="H70" t="s">
         <v>72</v>
       </c>
-      <c r="H70" t="s">
-        <v>73</v>
-      </c>
       <c r="I70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3470,25 +3476,25 @@
         <v>221</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G71" t="s">
+        <v>71</v>
+      </c>
+      <c r="H71" t="s">
         <v>72</v>
       </c>
-      <c r="H71" t="s">
-        <v>73</v>
-      </c>
       <c r="I71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3496,25 +3502,25 @@
         <v>222</v>
       </c>
       <c r="B72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G72" t="s">
+        <v>71</v>
+      </c>
+      <c r="H72" t="s">
         <v>72</v>
       </c>
-      <c r="H72" t="s">
-        <v>73</v>
-      </c>
       <c r="I72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3522,25 +3528,25 @@
         <v>223</v>
       </c>
       <c r="B73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G73" t="s">
+        <v>71</v>
+      </c>
+      <c r="H73" t="s">
         <v>72</v>
       </c>
-      <c r="H73" t="s">
-        <v>73</v>
-      </c>
       <c r="I73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3548,25 +3554,25 @@
         <v>224</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G74" t="s">
+        <v>71</v>
+      </c>
+      <c r="H74" t="s">
         <v>72</v>
       </c>
-      <c r="H74" t="s">
-        <v>73</v>
-      </c>
       <c r="I74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3574,25 +3580,25 @@
         <v>225</v>
       </c>
       <c r="B75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E75" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G75" t="s">
+        <v>71</v>
+      </c>
+      <c r="H75" t="s">
         <v>72</v>
       </c>
-      <c r="H75" t="s">
-        <v>73</v>
-      </c>
       <c r="I75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3600,25 +3606,25 @@
         <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G76" t="s">
+        <v>71</v>
+      </c>
+      <c r="H76" t="s">
         <v>72</v>
       </c>
-      <c r="H76" t="s">
-        <v>73</v>
-      </c>
       <c r="I76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3626,25 +3632,25 @@
         <v>227</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G77" t="s">
+        <v>71</v>
+      </c>
+      <c r="H77" t="s">
         <v>72</v>
       </c>
-      <c r="H77" t="s">
-        <v>73</v>
-      </c>
       <c r="I77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3652,25 +3658,25 @@
         <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E78" t="s">
         <v>229</v>
       </c>
       <c r="F78" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G78" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H78" t="s">
         <v>230</v>
       </c>
       <c r="I78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3678,25 +3684,25 @@
         <v>231</v>
       </c>
       <c r="B79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H79" t="s">
         <v>232</v>
       </c>
       <c r="I79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -3704,25 +3710,25 @@
         <v>233</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H80" t="s">
         <v>234</v>
       </c>
       <c r="I80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3730,25 +3736,25 @@
         <v>235</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H81" t="s">
         <v>234</v>
       </c>
       <c r="I81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3756,25 +3762,25 @@
         <v>236</v>
       </c>
       <c r="B82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E82" t="s">
         <v>229</v>
       </c>
       <c r="F82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G82" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H82" t="s">
         <v>230</v>
       </c>
       <c r="I82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3782,25 +3788,25 @@
         <v>237</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E83" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G83" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H83" t="s">
         <v>238</v>
       </c>
       <c r="I83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3808,25 +3814,25 @@
         <v>239</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H84" t="s">
         <v>240</v>
       </c>
       <c r="I84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3834,25 +3840,25 @@
         <v>241</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E85" t="s">
         <v>242</v>
       </c>
       <c r="F85" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G85" t="s">
+        <v>71</v>
+      </c>
+      <c r="H85" t="s">
         <v>72</v>
       </c>
-      <c r="H85" t="s">
-        <v>73</v>
-      </c>
       <c r="I85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3860,25 +3866,25 @@
         <v>243</v>
       </c>
       <c r="B86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E86" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F86" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G86" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H86" t="s">
         <v>244</v>
       </c>
       <c r="I86" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3886,25 +3892,25 @@
         <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" t="s">
         <v>246</v>
       </c>
       <c r="F87" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G87" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H87" t="s">
         <v>247</v>
       </c>
       <c r="I87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -3912,25 +3918,25 @@
         <v>248</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E88" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F88" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G88" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H88" t="s">
         <v>249</v>
       </c>
       <c r="I88" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -3938,25 +3944,25 @@
         <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E89" t="s">
         <v>251</v>
       </c>
       <c r="F89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G89" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H89" t="s">
         <v>252</v>
       </c>
       <c r="I89" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -3964,25 +3970,25 @@
         <v>253</v>
       </c>
       <c r="B90" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C90" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E90" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F90" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G90" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3990,25 +3996,25 @@
         <v>254</v>
       </c>
       <c r="B91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E91" t="s">
         <v>255</v>
       </c>
       <c r="F91" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G91" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H91" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I91" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -4016,25 +4022,25 @@
         <v>256</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E92" t="s">
         <v>255</v>
       </c>
       <c r="F92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G92" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H92" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -4042,25 +4048,25 @@
         <v>257</v>
       </c>
       <c r="B93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G93" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -4068,25 +4074,25 @@
         <v>258</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E94" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F94" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G94" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H94" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I94" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -4094,25 +4100,25 @@
         <v>259</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G95" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H95" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I95" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -4120,25 +4126,25 @@
         <v>260</v>
       </c>
       <c r="B96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E96" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H96" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -4146,25 +4152,25 @@
         <v>261</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E97" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F97" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H97" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4172,25 +4178,25 @@
         <v>262</v>
       </c>
       <c r="B98" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C98" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E98" t="s">
         <v>255</v>
       </c>
       <c r="F98" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G98" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I98" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4198,25 +4204,25 @@
         <v>263</v>
       </c>
       <c r="B99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E99" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G99" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H99" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I99" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4224,25 +4230,25 @@
         <v>264</v>
       </c>
       <c r="B100" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C100" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F100" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G100" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H100" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I100" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4250,25 +4256,25 @@
         <v>265</v>
       </c>
       <c r="B101" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C101" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F101" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G101" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H101" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I101" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4276,25 +4282,25 @@
         <v>266</v>
       </c>
       <c r="B102" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C102" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F102" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G102" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4302,25 +4308,25 @@
         <v>267</v>
       </c>
       <c r="B103" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C103" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E103" t="s">
         <v>229</v>
       </c>
       <c r="F103" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G103" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H103" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I103" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -4328,25 +4334,25 @@
         <v>268</v>
       </c>
       <c r="B104" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C104" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E104" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F104" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G104" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H104" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I104" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -4354,48 +4360,51 @@
         <v>269</v>
       </c>
       <c r="B105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E105" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G105" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I105" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>270</v>
       </c>
+      <c r="B106" t="s">
+        <v>68</v>
+      </c>
       <c r="C106" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F106" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G106" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I106" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>